<commit_message>
Menu de dudas en loop arreglado
</commit_message>
<xml_diff>
--- a/Wassauto/Excels/3resentrega_Only_Data .xlsx
+++ b/Wassauto/Excels/3resentrega_Only_Data .xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="416">
   <si>
     <t>LISTADO DE ENTREGAS</t>
   </si>
@@ -25,457 +25,460 @@
     <t>D3</t>
   </si>
   <si>
+    <t>CO11707029</t>
+  </si>
+  <si>
+    <t>DANIEL CORUJEIRA</t>
+  </si>
+  <si>
+    <t>TURQUESA</t>
+  </si>
+  <si>
+    <t>13:15</t>
+  </si>
+  <si>
+    <t>13:16</t>
+  </si>
+  <si>
+    <t>HOTELPTO</t>
+  </si>
+  <si>
+    <t>VW POLO</t>
+  </si>
+  <si>
+    <t>6507 GXJ</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(YARIS)  </t>
+  </si>
+  <si>
+    <t>Telf.: +34671152525</t>
+  </si>
+  <si>
+    <t>OFI RESERVA :</t>
+  </si>
+  <si>
+    <t>USUARIO CREACIÓN :</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>FECHA RESERVA :</t>
+  </si>
+  <si>
+    <t>H. RES. :</t>
+  </si>
+  <si>
+    <t>09:41</t>
+  </si>
+  <si>
+    <t>BLANCO</t>
+  </si>
+  <si>
+    <t>daniel#corujeira.es</t>
+  </si>
+  <si>
+    <t>Última Devolución:  :</t>
+  </si>
+  <si>
+    <t>CO1707086</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lugar: </t>
+  </si>
+  <si>
+    <t>GARAJE</t>
+  </si>
+  <si>
+    <t>TRIANFLOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fecha: </t>
+  </si>
+  <si>
+    <t>VE11707057</t>
+  </si>
+  <si>
+    <t>ALAMO OLIVER</t>
+  </si>
+  <si>
+    <t>SAN TELMO 211</t>
+  </si>
+  <si>
+    <t>09:30</t>
+  </si>
+  <si>
+    <t>08:00</t>
+  </si>
+  <si>
+    <t>PARKING</t>
+  </si>
+  <si>
+    <t>CITROEN C3</t>
+  </si>
+  <si>
+    <t>2735 LSY</t>
+  </si>
+  <si>
+    <t>VE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telf.: +34664580996 </t>
+  </si>
+  <si>
+    <t>18:42</t>
+  </si>
+  <si>
+    <t>GRIS</t>
+  </si>
+  <si>
+    <t>CO17070082</t>
+  </si>
+  <si>
+    <t>REINA SOFIA</t>
+  </si>
+  <si>
+    <t>EL MEDANO, PRIVADO</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>VE11708001</t>
+  </si>
+  <si>
+    <t>ALE</t>
+  </si>
+  <si>
+    <t>SAN FELIPE 203</t>
+  </si>
+  <si>
+    <t>VENEZUELA</t>
+  </si>
+  <si>
+    <t>9340 LML</t>
+  </si>
+  <si>
+    <t>Telf.: 669968954</t>
+  </si>
+  <si>
+    <t>10:00</t>
+  </si>
+  <si>
+    <t>VE17070059</t>
+  </si>
+  <si>
+    <t>EL TOPE 101</t>
+  </si>
+  <si>
+    <t>VE11708003</t>
+  </si>
+  <si>
+    <t>PARILLO CARLO</t>
+  </si>
+  <si>
+    <t>VALLE MAR 326</t>
+  </si>
+  <si>
+    <t>7032 HFP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telf.: +393293299445  </t>
+  </si>
+  <si>
+    <t>11:32</t>
+  </si>
+  <si>
+    <t>VE17070056</t>
+  </si>
+  <si>
+    <t>SAN TELMO 315</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>CO11706250</t>
+  </si>
+  <si>
+    <t>BERTAUT QUENTIN</t>
+  </si>
+  <si>
+    <t>BE LIVE EXPERIENCE OROTAVA</t>
+  </si>
+  <si>
+    <t>19:00</t>
+  </si>
+  <si>
+    <t>SEAT IBIZA</t>
+  </si>
+  <si>
+    <t>7839 HDW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(IBIZA)  COBRAR FIANZA  </t>
+  </si>
+  <si>
+    <t>Telf.: +33667970490  +33763204685</t>
+  </si>
+  <si>
+    <t>HE</t>
+  </si>
+  <si>
+    <t>11:03</t>
+  </si>
+  <si>
+    <t>CO17070098</t>
+  </si>
+  <si>
+    <t>BLUE SEA PUERTO RESORT</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>CO11706325</t>
+  </si>
+  <si>
+    <t>REGUERA WANDEN RAFAEL</t>
+  </si>
+  <si>
+    <t>PUERTO PALACE</t>
+  </si>
+  <si>
+    <t>TOYOTA YARIS</t>
+  </si>
+  <si>
+    <t>4128 HLL</t>
+  </si>
+  <si>
+    <t>ESPAÑOL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telf.: 667592812  </t>
+  </si>
+  <si>
+    <t>19:27</t>
+  </si>
+  <si>
+    <t>CO17070104</t>
+  </si>
+  <si>
+    <t>XIBANA PARK</t>
+  </si>
+  <si>
+    <t>QT11708000</t>
+  </si>
+  <si>
+    <t>BOTTICELLI MATTEO</t>
+  </si>
+  <si>
+    <t>LA QUINTA PARK</t>
+  </si>
+  <si>
+    <t>09:43</t>
+  </si>
+  <si>
+    <t>20:00</t>
+  </si>
+  <si>
+    <t>HOTELEXTRRAD</t>
+  </si>
+  <si>
+    <t>VW. POLO</t>
+  </si>
+  <si>
+    <t>7737 HXZ</t>
+  </si>
+  <si>
+    <t>INGLES</t>
+  </si>
+  <si>
+    <t>QT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telf.: 0039-3387654123  </t>
+  </si>
+  <si>
+    <t>BJ</t>
+  </si>
+  <si>
+    <t>CH17070013</t>
+  </si>
+  <si>
+    <t>TRIANFLOR 2220</t>
+  </si>
+  <si>
+    <t>EC11707017</t>
+  </si>
+  <si>
+    <t>BURNOG KRZYSZTOF</t>
+  </si>
+  <si>
+    <t>EL TOPE 526</t>
+  </si>
+  <si>
+    <t>2384 HTN</t>
+  </si>
+  <si>
+    <t>EC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telf.: +48725498564  </t>
+  </si>
+  <si>
+    <t>11:59</t>
+  </si>
+  <si>
+    <t>CO17070092</t>
+  </si>
+  <si>
+    <t>PQUE VACACIONAL EDEN</t>
+  </si>
+  <si>
+    <t>CH11708000</t>
+  </si>
+  <si>
+    <t>MARTIN HIERRO MANUEL</t>
+  </si>
+  <si>
+    <t>TRYP SN</t>
+  </si>
+  <si>
+    <t>2714 HTZ</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telf.: 655460585  </t>
+  </si>
+  <si>
+    <t>12:33</t>
+  </si>
+  <si>
+    <t>PLATA</t>
+  </si>
+  <si>
+    <t>ET17070009</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>CO11703298</t>
+  </si>
+  <si>
+    <t>CORADO FREITAS DIOGO</t>
+  </si>
+  <si>
+    <t>CONCORDIA</t>
+  </si>
+  <si>
+    <t>OFICINA INDEFINIDA *</t>
+  </si>
+  <si>
+    <t>7028 HFP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(UP)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telf.: 684363902  </t>
+  </si>
+  <si>
+    <t>09:25</t>
+  </si>
+  <si>
+    <t>diogo.corado#gmail.com</t>
+  </si>
+  <si>
+    <t>GE17070015</t>
+  </si>
+  <si>
+    <t>RODEOS</t>
+  </si>
+  <si>
+    <t>MIRAMAR 908</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>CO11706082</t>
+  </si>
+  <si>
+    <t>KUHLMANN FRANK</t>
+  </si>
+  <si>
+    <t>TROVADOR</t>
+  </si>
+  <si>
+    <t>GARAJE *</t>
+  </si>
+  <si>
+    <t>OPEL CORSA</t>
+  </si>
+  <si>
+    <t>8846 HYC</t>
+  </si>
+  <si>
+    <t>Telf.: +491715084197  +4915126425330</t>
+  </si>
+  <si>
+    <t>10:18</t>
+  </si>
+  <si>
+    <t>CO17070089</t>
+  </si>
+  <si>
+    <t>BEST SEMIRAMIS</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>CO11708005</t>
+  </si>
+  <si>
+    <t>GOLEADO BOIX MANUEL VICENTE</t>
+  </si>
+  <si>
+    <t>HOTEL PUERTO DE LA CRUZ 218</t>
+  </si>
+  <si>
+    <t>VW CADDY</t>
+  </si>
+  <si>
+    <t>0849 JBD</t>
+  </si>
+  <si>
+    <t>Telf.: 669821334  600394501</t>
+  </si>
+  <si>
+    <t>09:16</t>
+  </si>
+  <si>
+    <t>CH17070012</t>
+  </si>
+  <si>
+    <t>HOTELPTO FIANZA</t>
+  </si>
+  <si>
+    <t>SAN ANTONIO 1102</t>
+  </si>
+  <si>
     <t>CO11707086</t>
-  </si>
-  <si>
-    <t>DANIEL CORUJEIRA</t>
-  </si>
-  <si>
-    <t>TURQUESA</t>
-  </si>
-  <si>
-    <t>13:15</t>
-  </si>
-  <si>
-    <t>13:16</t>
-  </si>
-  <si>
-    <t>HOTELPTO</t>
-  </si>
-  <si>
-    <t>VW POLO</t>
-  </si>
-  <si>
-    <t>6507 GXJ</t>
-  </si>
-  <si>
-    <t>CO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(YARIS)  </t>
-  </si>
-  <si>
-    <t>Telf.: +34671152525</t>
-  </si>
-  <si>
-    <t>OFI RESERVA :</t>
-  </si>
-  <si>
-    <t>USUARIO CREACIÓN :</t>
-  </si>
-  <si>
-    <t>CA</t>
-  </si>
-  <si>
-    <t>FECHA RESERVA :</t>
-  </si>
-  <si>
-    <t>H. RES. :</t>
-  </si>
-  <si>
-    <t>09:41</t>
-  </si>
-  <si>
-    <t>BLANCO</t>
-  </si>
-  <si>
-    <t>daniel#corujeira.es</t>
-  </si>
-  <si>
-    <t>Última Devolución:  :</t>
-  </si>
-  <si>
-    <t>CO1707086</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lugar: </t>
-  </si>
-  <si>
-    <t>GARAJE</t>
-  </si>
-  <si>
-    <t>TRIANFLOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fecha: </t>
-  </si>
-  <si>
-    <t>VE11707057</t>
-  </si>
-  <si>
-    <t>ALAMO OLIVER</t>
-  </si>
-  <si>
-    <t>SAN TELMO 211</t>
-  </si>
-  <si>
-    <t>09:30</t>
-  </si>
-  <si>
-    <t>08:00</t>
-  </si>
-  <si>
-    <t>PARKING</t>
-  </si>
-  <si>
-    <t>CITROEN C3</t>
-  </si>
-  <si>
-    <t>2735 LSY</t>
-  </si>
-  <si>
-    <t>VE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telf.: +34664580996 </t>
-  </si>
-  <si>
-    <t>18:42</t>
-  </si>
-  <si>
-    <t>GRIS</t>
-  </si>
-  <si>
-    <t>CO17070082</t>
-  </si>
-  <si>
-    <t>REINA SOFIA</t>
-  </si>
-  <si>
-    <t>EL MEDANO, PRIVADO</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>VE11708001</t>
-  </si>
-  <si>
-    <t>ALE</t>
-  </si>
-  <si>
-    <t>SAN FELIPE 203</t>
-  </si>
-  <si>
-    <t>VENEZUELA</t>
-  </si>
-  <si>
-    <t>9340 LML</t>
-  </si>
-  <si>
-    <t>Telf.: 669968954</t>
-  </si>
-  <si>
-    <t>10:00</t>
-  </si>
-  <si>
-    <t>VE17070059</t>
-  </si>
-  <si>
-    <t>EL TOPE 101</t>
-  </si>
-  <si>
-    <t>VE11708003</t>
-  </si>
-  <si>
-    <t>PARILLO CARLO</t>
-  </si>
-  <si>
-    <t>VALLE MAR 326</t>
-  </si>
-  <si>
-    <t>7032 HFP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telf.: +393293299445  </t>
-  </si>
-  <si>
-    <t>11:32</t>
-  </si>
-  <si>
-    <t>VE17070056</t>
-  </si>
-  <si>
-    <t>SAN TELMO 315</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>CO11706250</t>
-  </si>
-  <si>
-    <t>BERTAUT QUENTIN</t>
-  </si>
-  <si>
-    <t>BE LIVE EXPERIENCE OROTAVA</t>
-  </si>
-  <si>
-    <t>19:00</t>
-  </si>
-  <si>
-    <t>SEAT IBIZA</t>
-  </si>
-  <si>
-    <t>7839 HDW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(IBIZA)  COBRAR FIANZA  </t>
-  </si>
-  <si>
-    <t>Telf.: +33667970490  +33763204685</t>
-  </si>
-  <si>
-    <t>HE</t>
-  </si>
-  <si>
-    <t>11:03</t>
-  </si>
-  <si>
-    <t>CO17070098</t>
-  </si>
-  <si>
-    <t>BLUE SEA PUERTO RESORT</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>CO11706325</t>
-  </si>
-  <si>
-    <t>REGUERA WANDEN RAFAEL</t>
-  </si>
-  <si>
-    <t>PUERTO PALACE</t>
-  </si>
-  <si>
-    <t>TOYOTA YARIS</t>
-  </si>
-  <si>
-    <t>4128 HLL</t>
-  </si>
-  <si>
-    <t>ESPAÑOL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telf.: 667592812  </t>
-  </si>
-  <si>
-    <t>19:27</t>
-  </si>
-  <si>
-    <t>CO17070104</t>
-  </si>
-  <si>
-    <t>XIBANA PARK</t>
-  </si>
-  <si>
-    <t>QT11708000</t>
-  </si>
-  <si>
-    <t>BOTTICELLI MATTEO</t>
-  </si>
-  <si>
-    <t>LA QUINTA PARK</t>
-  </si>
-  <si>
-    <t>09:43</t>
-  </si>
-  <si>
-    <t>20:00</t>
-  </si>
-  <si>
-    <t>HOTELEXTRRAD</t>
-  </si>
-  <si>
-    <t>VW. POLO</t>
-  </si>
-  <si>
-    <t>7737 HXZ</t>
-  </si>
-  <si>
-    <t>INGLES</t>
-  </si>
-  <si>
-    <t>QT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telf.: 0039-3387654123  </t>
-  </si>
-  <si>
-    <t>BJ</t>
-  </si>
-  <si>
-    <t>CH17070013</t>
-  </si>
-  <si>
-    <t>TRIANFLOR 2220</t>
-  </si>
-  <si>
-    <t>EC11707017</t>
-  </si>
-  <si>
-    <t>BURNOG KRZYSZTOF</t>
-  </si>
-  <si>
-    <t>EL TOPE 526</t>
-  </si>
-  <si>
-    <t>2384 HTN</t>
-  </si>
-  <si>
-    <t>EC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telf.: +48725498564  </t>
-  </si>
-  <si>
-    <t>11:59</t>
-  </si>
-  <si>
-    <t>CO17070092</t>
-  </si>
-  <si>
-    <t>PQUE VACACIONAL EDEN</t>
-  </si>
-  <si>
-    <t>CH11708000</t>
-  </si>
-  <si>
-    <t>MARTIN HIERRO MANUEL</t>
-  </si>
-  <si>
-    <t>TRYP SN</t>
-  </si>
-  <si>
-    <t>2714 HTZ</t>
-  </si>
-  <si>
-    <t>CH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telf.: 655460585  </t>
-  </si>
-  <si>
-    <t>12:33</t>
-  </si>
-  <si>
-    <t>PLATA</t>
-  </si>
-  <si>
-    <t>ET17070009</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>CO11703298</t>
-  </si>
-  <si>
-    <t>CORADO FREITAS DIOGO</t>
-  </si>
-  <si>
-    <t>CONCORDIA</t>
-  </si>
-  <si>
-    <t>OFICINA INDEFINIDA *</t>
-  </si>
-  <si>
-    <t>7028 HFP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(UP)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telf.: 684363902  </t>
-  </si>
-  <si>
-    <t>09:25</t>
-  </si>
-  <si>
-    <t>diogo.corado#gmail.com</t>
-  </si>
-  <si>
-    <t>GE17070015</t>
-  </si>
-  <si>
-    <t>RODEOS</t>
-  </si>
-  <si>
-    <t>MIRAMAR 908</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>CO11706082</t>
-  </si>
-  <si>
-    <t>KUHLMANN FRANK</t>
-  </si>
-  <si>
-    <t>TROVADOR</t>
-  </si>
-  <si>
-    <t>GARAJE *</t>
-  </si>
-  <si>
-    <t>OPEL CORSA</t>
-  </si>
-  <si>
-    <t>8846 HYC</t>
-  </si>
-  <si>
-    <t>Telf.: +491715084197  +4915126425330</t>
-  </si>
-  <si>
-    <t>10:18</t>
-  </si>
-  <si>
-    <t>CO17070089</t>
-  </si>
-  <si>
-    <t>BEST SEMIRAMIS</t>
-  </si>
-  <si>
-    <t>H3</t>
-  </si>
-  <si>
-    <t>CO11708005</t>
-  </si>
-  <si>
-    <t>GOLEADO BOIX MANUEL VICENTE</t>
-  </si>
-  <si>
-    <t>HOTEL PUERTO DE LA CRUZ 218</t>
-  </si>
-  <si>
-    <t>VW CADDY</t>
-  </si>
-  <si>
-    <t>0849 JBD</t>
-  </si>
-  <si>
-    <t>Telf.: 669821334  600394501</t>
-  </si>
-  <si>
-    <t>09:16</t>
-  </si>
-  <si>
-    <t>CH17070012</t>
-  </si>
-  <si>
-    <t>HOTELPTO FIANZA</t>
-  </si>
-  <si>
-    <t>SAN ANTONIO 1102</t>
   </si>
   <si>
     <t>MENDAÑA TROTTER ALFREDO</t>
@@ -4054,10 +4057,10 @@
         <v>133</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>4</v>
+        <v>155</v>
       </c>
       <c r="C27" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D27" t="s" s="2">
         <v>109</v>
@@ -4066,7 +4069,7 @@
         <v>42961</v>
       </c>
       <c r="F27" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G27" s="3">
         <v>42966</v>
@@ -4084,11 +4087,11 @@
         <v>138</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="M27" s="4"/>
       <c r="N27" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="O27" t="s" s="2">
         <v>12</v>
@@ -4097,11 +4100,11 @@
         <v>12</v>
       </c>
       <c r="Q27" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="R27" s="4"/>
       <c r="S27" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="T27" t="s" s="2">
         <v>15</v>
@@ -4125,10 +4128,10 @@
         <v>19</v>
       </c>
       <c r="AA27" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AB27" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="28" ht="12.75" customHeight="1">
@@ -4137,7 +4140,7 @@
         <v>23</v>
       </c>
       <c r="C28" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D28" t="s" s="2">
         <v>25</v>
@@ -4146,7 +4149,7 @@
         <v>26</v>
       </c>
       <c r="F28" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G28" t="s" s="2">
         <v>28</v>
@@ -4182,19 +4185,19 @@
         <v>45</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C29" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D29" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E29" s="3">
         <v>42961</v>
       </c>
       <c r="F29" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G29" s="3">
         <v>42963</v>
@@ -4212,11 +4215,11 @@
         <v>10</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="M29" s="4"/>
       <c r="N29" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="O29" t="s" s="2">
         <v>12</v>
@@ -4225,11 +4228,11 @@
         <v>12</v>
       </c>
       <c r="Q29" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="R29" s="4"/>
       <c r="S29" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="T29" t="s" s="2">
         <v>15</v>
@@ -4253,7 +4256,7 @@
         <v>19</v>
       </c>
       <c r="AA29" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AB29" t="s" s="2">
         <v>21</v>
@@ -4265,7 +4268,7 @@
         <v>23</v>
       </c>
       <c r="C30" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D30" t="s" s="2">
         <v>25</v>
@@ -4274,7 +4277,7 @@
         <v>26</v>
       </c>
       <c r="F30" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G30" t="s" s="2">
         <v>28</v>
@@ -4310,25 +4313,25 @@
         <v>63</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C31" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D31" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E31" s="3">
         <v>42961</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G31" s="3">
         <v>42966</v>
       </c>
       <c r="H31" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I31" s="5">
         <v>5</v>
@@ -4340,13 +4343,13 @@
         <v>68</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="M31" t="s" s="2">
         <v>82</v>
       </c>
       <c r="N31" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="O31" t="s" s="2">
         <v>12</v>
@@ -4355,11 +4358,11 @@
         <v>12</v>
       </c>
       <c r="Q31" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="R31" s="4"/>
       <c r="S31" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="T31" t="s" s="2">
         <v>15</v>
@@ -4383,7 +4386,7 @@
         <v>19</v>
       </c>
       <c r="AA31" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AB31" t="s" s="2">
         <v>21</v>
@@ -4395,7 +4398,7 @@
         <v>23</v>
       </c>
       <c r="C32" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D32" t="s" s="2">
         <v>25</v>
@@ -4404,7 +4407,7 @@
         <v>92</v>
       </c>
       <c r="F32" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G32" t="s" s="2">
         <v>28</v>
@@ -4440,19 +4443,19 @@
         <v>76</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C33" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D33" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E33" s="3">
         <v>42961</v>
       </c>
       <c r="F33" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G33" s="3">
         <v>42965</v>
@@ -4470,11 +4473,11 @@
         <v>80</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="M33" s="4"/>
       <c r="N33" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O33" t="s" s="2">
         <v>114</v>
@@ -4487,7 +4490,7 @@
       </c>
       <c r="R33" s="4"/>
       <c r="S33" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="T33" t="s" s="2">
         <v>15</v>
@@ -4511,10 +4514,10 @@
         <v>19</v>
       </c>
       <c r="AA33" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AB33" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="34" ht="12.75" customHeight="1">
@@ -4523,7 +4526,7 @@
         <v>23</v>
       </c>
       <c r="C34" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D34" t="s" s="2">
         <v>25</v>
@@ -4532,7 +4535,7 @@
         <v>34</v>
       </c>
       <c r="F34" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G34" t="s" s="2">
         <v>28</v>
@@ -4568,41 +4571,41 @@
         <v>45</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C35" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D35" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E35" s="3">
         <v>42961</v>
       </c>
       <c r="F35" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G35" s="3">
         <v>42965</v>
       </c>
       <c r="H35" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I35" s="5">
         <v>4</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="K35" t="s" s="2">
         <v>10</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="M35" s="4"/>
       <c r="N35" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="O35" t="s" s="2">
         <v>37</v>
@@ -4615,7 +4618,7 @@
       </c>
       <c r="R35" s="4"/>
       <c r="S35" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="T35" t="s" s="2">
         <v>15</v>
@@ -4651,7 +4654,7 @@
         <v>23</v>
       </c>
       <c r="C36" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D36" t="s" s="2">
         <v>25</v>
@@ -4660,7 +4663,7 @@
         <v>131</v>
       </c>
       <c r="F36" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G36" t="s" s="2">
         <v>28</v>
@@ -4696,19 +4699,19 @@
         <v>76</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C37" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D37" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E37" s="3">
         <v>42961</v>
       </c>
       <c r="F37" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="G37" s="3">
         <v>42967</v>
@@ -4720,38 +4723,38 @@
         <v>7</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="K37" t="s" s="2">
         <v>80</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="M37" t="s" s="2">
         <v>82</v>
       </c>
       <c r="N37" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="O37" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="P37" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="Q37" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="R37" s="4"/>
       <c r="S37" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="T37" t="s" s="2">
         <v>15</v>
       </c>
       <c r="U37" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="V37" t="s" s="2">
         <v>16</v>
@@ -4769,7 +4772,7 @@
         <v>19</v>
       </c>
       <c r="AA37" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="AB37" t="s" s="2">
         <v>117</v>
@@ -4777,13 +4780,13 @@
     </row>
     <row r="38" ht="12.75" customHeight="1">
       <c r="A38" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B38" t="s" s="2">
         <v>23</v>
       </c>
       <c r="C38" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D38" t="s" s="2">
         <v>25</v>
@@ -4792,7 +4795,7 @@
         <v>9</v>
       </c>
       <c r="F38" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="G38" t="s" s="2">
         <v>28</v>
@@ -4825,28 +4828,28 @@
     </row>
     <row r="39" ht="12.75" customHeight="1">
       <c r="A39" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C39" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D39" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E39" s="3">
         <v>42961</v>
       </c>
       <c r="F39" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G39" s="3">
         <v>42964</v>
       </c>
       <c r="H39" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I39" s="5">
         <v>3</v>
@@ -4855,14 +4858,14 @@
         <v>9</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="M39" s="4"/>
       <c r="N39" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>12</v>
@@ -4871,11 +4874,11 @@
         <v>12</v>
       </c>
       <c r="Q39" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="R39" s="4"/>
       <c r="S39" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="T39" t="s" s="2">
         <v>15</v>
@@ -4899,7 +4902,7 @@
         <v>19</v>
       </c>
       <c r="AA39" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="AB39" t="s" s="2">
         <v>21</v>
@@ -4911,7 +4914,7 @@
         <v>23</v>
       </c>
       <c r="C40" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D40" t="s" s="2">
         <v>25</v>
@@ -4920,7 +4923,7 @@
         <v>43</v>
       </c>
       <c r="F40" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="G40" t="s" s="2">
         <v>28</v>
@@ -4956,10 +4959,10 @@
         <v>63</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C41" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D41" t="s" s="2">
         <v>143</v>
@@ -4986,11 +4989,11 @@
         <v>68</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="M41" s="4"/>
       <c r="N41" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="O41" t="s" s="2">
         <v>12</v>
@@ -4999,11 +5002,11 @@
         <v>12</v>
       </c>
       <c r="Q41" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="R41" s="4"/>
       <c r="S41" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="T41" t="s" s="2">
         <v>15</v>
@@ -5027,7 +5030,7 @@
         <v>19</v>
       </c>
       <c r="AA41" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="AB41" t="s" s="2">
         <v>21</v>
@@ -5039,7 +5042,7 @@
         <v>23</v>
       </c>
       <c r="C42" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D42" t="s" s="2">
         <v>25</v>
@@ -5048,7 +5051,7 @@
         <v>43</v>
       </c>
       <c r="F42" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="G42" t="s" s="2">
         <v>28</v>
@@ -5084,25 +5087,25 @@
         <v>45</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C43" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D43" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E43" s="3">
         <v>42961</v>
       </c>
       <c r="F43" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G43" s="3">
         <v>42971</v>
       </c>
       <c r="H43" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="I43" s="5">
         <v>10</v>
@@ -5114,11 +5117,11 @@
         <v>10</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="M43" s="4"/>
       <c r="N43" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="O43" t="s" s="2">
         <v>12</v>
@@ -5127,11 +5130,11 @@
         <v>12</v>
       </c>
       <c r="Q43" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="R43" s="4"/>
       <c r="S43" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="T43" t="s" s="2">
         <v>15</v>
@@ -5155,7 +5158,7 @@
         <v>19</v>
       </c>
       <c r="AA43" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="AB43" t="s" s="2">
         <v>21</v>
@@ -5163,13 +5166,13 @@
     </row>
     <row r="44" ht="12.75" customHeight="1">
       <c r="A44" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B44" t="s" s="2">
         <v>23</v>
       </c>
       <c r="C44" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D44" t="s" s="2">
         <v>25</v>
@@ -5178,7 +5181,7 @@
         <v>26</v>
       </c>
       <c r="F44" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="G44" t="s" s="2">
         <v>28</v>
@@ -5214,25 +5217,25 @@
         <v>76</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C45" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D45" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E45" s="3">
         <v>42961</v>
       </c>
       <c r="F45" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="G45" s="3">
         <v>42971</v>
       </c>
       <c r="H45" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="I45" s="5">
         <v>10</v>
@@ -5244,11 +5247,11 @@
         <v>68</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="M45" s="4"/>
       <c r="N45" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="O45" t="s" s="2">
         <v>37</v>
@@ -5261,7 +5264,7 @@
       </c>
       <c r="R45" s="4"/>
       <c r="S45" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="T45" t="s" s="2">
         <v>15</v>
@@ -5285,7 +5288,7 @@
         <v>19</v>
       </c>
       <c r="AA45" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AB45" t="s" s="2">
         <v>21</v>
@@ -5293,13 +5296,13 @@
     </row>
     <row r="46" ht="12.75" customHeight="1">
       <c r="A46" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B46" t="s" s="2">
         <v>23</v>
       </c>
       <c r="C46" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D46" t="s" s="2">
         <v>25</v>
@@ -5308,7 +5311,7 @@
         <v>9</v>
       </c>
       <c r="F46" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="G46" t="s" s="2">
         <v>28</v>
@@ -5344,13 +5347,13 @@
         <v>45</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C47" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D47" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E47" s="3">
         <v>42962</v>
@@ -5374,13 +5377,13 @@
         <v>93</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="M47" t="s" s="2">
         <v>82</v>
       </c>
       <c r="N47" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="O47" t="s" s="2">
         <v>96</v>
@@ -5393,7 +5396,7 @@
       </c>
       <c r="R47" s="4"/>
       <c r="S47" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="T47" t="s" s="2">
         <v>15</v>
@@ -5417,7 +5420,7 @@
         <v>19</v>
       </c>
       <c r="AA47" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AB47" t="s" s="2">
         <v>21</v>
@@ -5429,7 +5432,7 @@
         <v>23</v>
       </c>
       <c r="C48" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D48" t="s" s="2">
         <v>25</v>
@@ -5474,13 +5477,13 @@
         <v>45</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C49" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D49" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="E49" s="3">
         <v>42962</v>
@@ -5504,11 +5507,11 @@
         <v>10</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="M49" s="4"/>
       <c r="N49" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="O49" t="s" s="2">
         <v>12</v>
@@ -5517,11 +5520,11 @@
         <v>12</v>
       </c>
       <c r="Q49" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="R49" s="4"/>
       <c r="S49" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="T49" t="s" s="2">
         <v>15</v>
@@ -5545,7 +5548,7 @@
         <v>19</v>
       </c>
       <c r="AA49" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="AB49" t="s" s="2">
         <v>21</v>
@@ -5557,7 +5560,7 @@
         <v>23</v>
       </c>
       <c r="C50" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D50" t="s" s="2">
         <v>25</v>
@@ -5566,7 +5569,7 @@
         <v>34</v>
       </c>
       <c r="F50" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="G50" t="s" s="2">
         <v>28</v>
@@ -5602,13 +5605,13 @@
         <v>63</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C51" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D51" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="E51" s="3">
         <v>42962</v>
@@ -5632,11 +5635,11 @@
         <v>68</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="M51" s="4"/>
       <c r="N51" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>37</v>
@@ -5649,7 +5652,7 @@
       </c>
       <c r="R51" s="4"/>
       <c r="S51" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="T51" t="s" s="2">
         <v>15</v>
@@ -5673,7 +5676,7 @@
         <v>19</v>
       </c>
       <c r="AA51" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="AB51" t="s" s="2">
         <v>21</v>
@@ -5685,7 +5688,7 @@
         <v>23</v>
       </c>
       <c r="C52" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D52" t="s" s="2">
         <v>25</v>
@@ -5694,7 +5697,7 @@
         <v>9</v>
       </c>
       <c r="F52" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="G52" t="s" s="2">
         <v>28</v>
@@ -5730,13 +5733,13 @@
         <v>45</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C53" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D53" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E53" s="3">
         <v>42962</v>
@@ -5760,11 +5763,11 @@
         <v>10</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="M53" s="4"/>
       <c r="N53" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="O53" t="s" s="2">
         <v>37</v>
@@ -5777,7 +5780,7 @@
       </c>
       <c r="R53" s="4"/>
       <c r="S53" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="T53" t="s" s="2">
         <v>15</v>
@@ -5801,7 +5804,7 @@
         <v>19</v>
       </c>
       <c r="AA53" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="AB53" t="s" s="2">
         <v>21</v>
@@ -5813,7 +5816,7 @@
         <v>23</v>
       </c>
       <c r="C54" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D54" t="s" s="2">
         <v>25</v>
@@ -5822,7 +5825,7 @@
         <v>9</v>
       </c>
       <c r="F54" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G54" t="s" s="2">
         <v>28</v>
@@ -5858,13 +5861,13 @@
         <v>45</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C55" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D55" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E55" s="3">
         <v>42962</v>
@@ -5882,17 +5885,17 @@
         <v>3</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="K55" t="s" s="2">
         <v>10</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="M55" s="4"/>
       <c r="N55" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="O55" t="s" s="2">
         <v>105</v>
@@ -5905,7 +5908,7 @@
       </c>
       <c r="R55" s="4"/>
       <c r="S55" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="T55" t="s" s="2">
         <v>15</v>
@@ -5929,7 +5932,7 @@
         <v>19</v>
       </c>
       <c r="AA55" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AB55" t="s" s="2">
         <v>21</v>
@@ -5941,16 +5944,16 @@
         <v>23</v>
       </c>
       <c r="C56" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D56" t="s" s="2">
         <v>25</v>
       </c>
       <c r="E56" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="F56" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="G56" t="s" s="2">
         <v>28</v>
@@ -5986,13 +5989,13 @@
         <v>63</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C57" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D57" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E57" s="3">
         <v>42962</v>
@@ -6010,7 +6013,7 @@
         <v>1</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="K57" t="s" s="2">
         <v>68</v>
@@ -6020,7 +6023,7 @@
       </c>
       <c r="M57" s="4"/>
       <c r="N57" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="O57" t="s" s="2">
         <v>105</v>
@@ -6033,7 +6036,7 @@
       </c>
       <c r="R57" s="4"/>
       <c r="S57" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="T57" t="s" s="2">
         <v>15</v>
@@ -6057,7 +6060,7 @@
         <v>19</v>
       </c>
       <c r="AA57" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="AB57" t="s" s="2">
         <v>21</v>
@@ -6114,13 +6117,13 @@
         <v>76</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C59" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D59" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E59" s="3">
         <v>42962</v>
@@ -6138,7 +6141,7 @@
         <v>3</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="K59" t="s" s="2">
         <v>80</v>
@@ -6148,7 +6151,7 @@
       </c>
       <c r="M59" s="4"/>
       <c r="N59" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="O59" t="s" s="2">
         <v>114</v>
@@ -6161,7 +6164,7 @@
       </c>
       <c r="R59" s="4"/>
       <c r="S59" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="T59" t="s" s="2">
         <v>15</v>
@@ -6185,7 +6188,7 @@
         <v>19</v>
       </c>
       <c r="AA59" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AB59" t="s" s="2">
         <v>6</v>
@@ -6242,13 +6245,13 @@
         <v>63</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C61" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D61" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E61" s="3">
         <v>42962</v>
@@ -6260,7 +6263,7 @@
         <v>42975</v>
       </c>
       <c r="H61" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="I61" s="5">
         <v>13</v>
@@ -6272,11 +6275,11 @@
         <v>68</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="M61" s="4"/>
       <c r="N61" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="O61" t="s" s="2">
         <v>114</v>
@@ -6289,7 +6292,7 @@
       </c>
       <c r="R61" s="4"/>
       <c r="S61" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="T61" t="s" s="2">
         <v>15</v>
@@ -6313,7 +6316,7 @@
         <v>19</v>
       </c>
       <c r="AA61" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="AB61" t="s" s="2">
         <v>21</v>
@@ -6325,7 +6328,7 @@
         <v>23</v>
       </c>
       <c r="C62" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D62" t="s" s="2">
         <v>25</v>
@@ -6334,7 +6337,7 @@
         <v>43</v>
       </c>
       <c r="F62" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="G62" t="s" s="2">
         <v>28</v>
@@ -6370,10 +6373,10 @@
         <v>76</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C63" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D63" t="s" s="2">
         <v>79</v>
@@ -6388,7 +6391,7 @@
         <v>42966</v>
       </c>
       <c r="H63" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="I63" s="5">
         <v>4</v>
@@ -6400,11 +6403,11 @@
         <v>80</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="M63" s="4"/>
       <c r="N63" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="O63" t="s" s="2">
         <v>12</v>
@@ -6417,7 +6420,7 @@
       </c>
       <c r="R63" s="4"/>
       <c r="S63" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="T63" t="s" s="2">
         <v>15</v>
@@ -6441,7 +6444,7 @@
         <v>19</v>
       </c>
       <c r="AA63" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="AB63" t="s" s="2">
         <v>6</v>
@@ -6453,7 +6456,7 @@
         <v>23</v>
       </c>
       <c r="C64" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D64" t="s" s="2">
         <v>25</v>
@@ -6498,13 +6501,13 @@
         <v>45</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C65" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D65" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="E65" s="3">
         <v>42962</v>
@@ -6516,7 +6519,7 @@
         <v>42967</v>
       </c>
       <c r="H65" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="I65" s="5">
         <v>5</v>
@@ -6528,13 +6531,13 @@
         <v>10</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="M65" t="s" s="2">
         <v>82</v>
       </c>
       <c r="N65" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="O65" t="s" s="2">
         <v>12</v>
@@ -6543,11 +6546,11 @@
         <v>12</v>
       </c>
       <c r="Q65" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="R65" s="4"/>
       <c r="S65" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="T65" t="s" s="2">
         <v>15</v>
@@ -6571,7 +6574,7 @@
         <v>19</v>
       </c>
       <c r="AA65" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="AB65" t="s" s="2">
         <v>41</v>
@@ -6583,7 +6586,7 @@
         <v>23</v>
       </c>
       <c r="C66" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D66" t="s" s="2">
         <v>25</v>
@@ -6592,7 +6595,7 @@
         <v>9</v>
       </c>
       <c r="F66" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="G66" t="s" s="2">
         <v>28</v>
@@ -6628,13 +6631,13 @@
         <v>45</v>
       </c>
       <c r="B67" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C67" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D67" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E67" s="3">
         <v>42962</v>
@@ -6658,13 +6661,13 @@
         <v>93</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="M67" t="s" s="2">
         <v>82</v>
       </c>
       <c r="N67" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="O67" t="s" s="2">
         <v>96</v>
@@ -6677,7 +6680,7 @@
       </c>
       <c r="R67" s="4"/>
       <c r="S67" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="T67" t="s" s="2">
         <v>15</v>
@@ -6701,7 +6704,7 @@
         <v>19</v>
       </c>
       <c r="AA67" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="AB67" t="s" s="2">
         <v>21</v>
@@ -6713,7 +6716,7 @@
         <v>23</v>
       </c>
       <c r="C68" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D68" t="s" s="2">
         <v>25</v>
@@ -6722,7 +6725,7 @@
         <v>34</v>
       </c>
       <c r="F68" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="G68" t="s" s="2">
         <v>28</v>
@@ -6758,19 +6761,19 @@
         <v>76</v>
       </c>
       <c r="B69" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C69" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D69" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E69" s="3">
         <v>42962</v>
       </c>
       <c r="F69" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="G69" s="3">
         <v>42964</v>
@@ -6788,32 +6791,32 @@
         <v>80</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="M69" t="s" s="2">
         <v>82</v>
       </c>
       <c r="N69" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="O69" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="P69" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="Q69" t="s" s="2">
         <v>38</v>
       </c>
       <c r="R69" s="4"/>
       <c r="S69" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="T69" t="s" s="2">
         <v>15</v>
       </c>
       <c r="U69" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="V69" t="s" s="2">
         <v>16</v>
@@ -6831,7 +6834,7 @@
         <v>19</v>
       </c>
       <c r="AA69" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="AB69" t="s" s="2">
         <v>21</v>
@@ -6843,7 +6846,7 @@
         <v>23</v>
       </c>
       <c r="C70" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D70" t="s" s="2">
         <v>25</v>
@@ -6852,7 +6855,7 @@
         <v>9</v>
       </c>
       <c r="F70" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="G70" t="s" s="2">
         <v>28</v>
@@ -6888,25 +6891,25 @@
         <v>45</v>
       </c>
       <c r="B71" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C71" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D71" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="E71" s="3">
         <v>42962</v>
       </c>
       <c r="F71" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G71" s="3">
         <v>42963</v>
       </c>
       <c r="H71" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I71" s="5">
         <v>1</v>
@@ -6918,11 +6921,11 @@
         <v>10</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="M71" s="4"/>
       <c r="N71" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="O71" t="s" s="2">
         <v>12</v>
@@ -6935,7 +6938,7 @@
       </c>
       <c r="R71" s="4"/>
       <c r="S71" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="T71" t="s" s="2">
         <v>15</v>
@@ -6959,7 +6962,7 @@
         <v>19</v>
       </c>
       <c r="AA71" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="AB71" t="s" s="2">
         <v>21</v>
@@ -6967,13 +6970,13 @@
     </row>
     <row r="72" ht="12.75" customHeight="1">
       <c r="A72" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B72" t="s" s="2">
         <v>23</v>
       </c>
       <c r="C72" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D72" t="s" s="2">
         <v>25</v>
@@ -6982,7 +6985,7 @@
         <v>9</v>
       </c>
       <c r="F72" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="G72" t="s" s="2">
         <v>28</v>
@@ -7018,19 +7021,19 @@
         <v>45</v>
       </c>
       <c r="B73" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C73" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D73" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="E73" s="3">
         <v>42962</v>
       </c>
       <c r="F73" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G73" s="3">
         <v>42968</v>
@@ -7042,15 +7045,15 @@
         <v>7</v>
       </c>
       <c r="J73" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="K73" s="4"/>
       <c r="L73" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="M73" s="4"/>
       <c r="N73" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="O73" t="s" s="2">
         <v>114</v>
@@ -7063,7 +7066,7 @@
       </c>
       <c r="R73" s="4"/>
       <c r="S73" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="T73" t="s" s="2">
         <v>15</v>
@@ -7087,7 +7090,7 @@
         <v>19</v>
       </c>
       <c r="AA73" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="AB73" t="s" s="2">
         <v>21</v>
@@ -7099,7 +7102,7 @@
         <v>23</v>
       </c>
       <c r="C74" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D74" t="s" s="2">
         <v>25</v>
@@ -7108,7 +7111,7 @@
         <v>131</v>
       </c>
       <c r="F74" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="G74" t="s" s="2">
         <v>28</v>
@@ -7144,41 +7147,41 @@
         <v>45</v>
       </c>
       <c r="B75" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C75" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D75" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="E75" s="3">
         <v>42962</v>
       </c>
       <c r="F75" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="G75" s="3">
         <v>42973</v>
       </c>
       <c r="H75" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="I75" s="5">
         <v>12</v>
       </c>
       <c r="J75" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="K75" t="s" s="2">
         <v>10</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="M75" s="4"/>
       <c r="N75" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="O75" t="s" s="2">
         <v>114</v>
@@ -7187,11 +7190,11 @@
         <v>114</v>
       </c>
       <c r="Q75" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="R75" s="4"/>
       <c r="S75" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="T75" t="s" s="2">
         <v>15</v>
@@ -7215,7 +7218,7 @@
         <v>19</v>
       </c>
       <c r="AA75" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AB75" t="s" s="2">
         <v>21</v>
@@ -7227,7 +7230,7 @@
         <v>23</v>
       </c>
       <c r="C76" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D76" t="s" s="2">
         <v>25</v>
@@ -7272,43 +7275,43 @@
         <v>63</v>
       </c>
       <c r="B77" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C77" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D77" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="E77" s="3">
         <v>42962</v>
       </c>
       <c r="F77" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G77" s="3">
         <v>42979</v>
       </c>
       <c r="H77" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="I77" s="5">
         <v>17</v>
       </c>
       <c r="J77" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="K77" t="s" s="2">
         <v>10</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="M77" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="N77" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="O77" t="s" s="2">
         <v>12</v>
@@ -7317,11 +7320,11 @@
         <v>12</v>
       </c>
       <c r="Q77" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="R77" s="4"/>
       <c r="S77" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="T77" t="s" s="2">
         <v>15</v>
@@ -7345,7 +7348,7 @@
         <v>19</v>
       </c>
       <c r="AA77" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="AB77" t="s" s="2">
         <v>21</v>
@@ -7353,13 +7356,13 @@
     </row>
     <row r="78" ht="12.75" customHeight="1">
       <c r="A78" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B78" t="s" s="2">
         <v>23</v>
       </c>
       <c r="C78" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="D78" t="s" s="2">
         <v>25</v>
@@ -7368,7 +7371,7 @@
         <v>34</v>
       </c>
       <c r="F78" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="G78" t="s" s="2">
         <v>28</v>
@@ -7404,19 +7407,19 @@
         <v>45</v>
       </c>
       <c r="B79" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C79" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D79" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="E79" s="3">
         <v>42962</v>
       </c>
       <c r="F79" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G79" s="3">
         <v>42969</v>
@@ -7432,11 +7435,11 @@
       </c>
       <c r="K79" s="4"/>
       <c r="L79" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="M79" s="4"/>
       <c r="N79" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="O79" t="s" s="2">
         <v>37</v>
@@ -7449,7 +7452,7 @@
       </c>
       <c r="R79" s="4"/>
       <c r="S79" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="T79" t="s" s="2">
         <v>15</v>
@@ -7473,7 +7476,7 @@
         <v>19</v>
       </c>
       <c r="AA79" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="AB79" t="s" s="2">
         <v>21</v>
@@ -7485,7 +7488,7 @@
         <v>23</v>
       </c>
       <c r="C80" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D80" t="s" s="2">
         <v>25</v>
@@ -7494,7 +7497,7 @@
         <v>26</v>
       </c>
       <c r="F80" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="G80" t="s" s="2">
         <v>28</v>
@@ -7530,19 +7533,19 @@
         <v>45</v>
       </c>
       <c r="B81" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C81" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D81" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="E81" s="3">
         <v>42962</v>
       </c>
       <c r="F81" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="G81" s="3">
         <v>42966</v>
@@ -7560,13 +7563,13 @@
         <v>10</v>
       </c>
       <c r="L81" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="M81" t="s" s="2">
         <v>82</v>
       </c>
       <c r="N81" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="O81" t="s" s="2">
         <v>12</v>
@@ -7575,11 +7578,11 @@
         <v>12</v>
       </c>
       <c r="Q81" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="R81" s="4"/>
       <c r="S81" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="T81" t="s" s="2">
         <v>15</v>
@@ -7603,7 +7606,7 @@
         <v>19</v>
       </c>
       <c r="AA81" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="AB81" t="s" s="2">
         <v>21</v>
@@ -7611,13 +7614,13 @@
     </row>
     <row r="82" ht="12.75" customHeight="1">
       <c r="A82" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B82" t="s" s="2">
         <v>23</v>
       </c>
       <c r="C82" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D82" t="s" s="2">
         <v>25</v>
@@ -7626,7 +7629,7 @@
         <v>9</v>
       </c>
       <c r="F82" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="G82" t="s" s="2">
         <v>28</v>
@@ -7662,25 +7665,25 @@
         <v>76</v>
       </c>
       <c r="B83" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C83" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D83" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E83" s="3">
         <v>42962</v>
       </c>
       <c r="F83" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="G83" s="3">
         <v>42978</v>
       </c>
       <c r="H83" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="I83" s="5">
         <v>16</v>
@@ -7692,11 +7695,11 @@
         <v>80</v>
       </c>
       <c r="L83" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="M83" s="4"/>
       <c r="N83" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="O83" t="s" s="2">
         <v>12</v>
@@ -7705,11 +7708,11 @@
         <v>12</v>
       </c>
       <c r="Q83" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="R83" s="4"/>
       <c r="S83" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="T83" t="s" s="2">
         <v>15</v>
@@ -7733,7 +7736,7 @@
         <v>19</v>
       </c>
       <c r="AA83" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="AB83" t="s" s="2">
         <v>117</v>
@@ -7741,13 +7744,13 @@
     </row>
     <row r="84" ht="12.75" customHeight="1">
       <c r="A84" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B84" t="s" s="2">
         <v>23</v>
       </c>
       <c r="C84" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D84" t="s" s="2">
         <v>25</v>
@@ -7756,7 +7759,7 @@
         <v>131</v>
       </c>
       <c r="F84" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="G84" t="s" s="2">
         <v>28</v>
@@ -7789,7 +7792,7 @@
     </row>
     <row r="85" ht="12.75" customHeight="1">
       <c r="A85" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B85" s="5">
         <v>41</v>
@@ -7823,7 +7826,7 @@
     </row>
     <row r="86" ht="12.75" customHeight="1">
       <c r="A86" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>

</xml_diff>